<commit_message>
avg sp/s for population
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -1804,7 +1804,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2081,7 +2081,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2329,7 +2329,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2354,13 +2354,13 @@
       <selection pane="topRight" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.42"/>
   </cols>
   <sheetData>
@@ -4066,15 +4066,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
   </cols>
@@ -4167,14 +4167,14 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>45198</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5065,11 +5065,11 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -6689,7 +6689,7 @@
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>

</xml_diff>

<commit_message>
updated metadata.xlsx -- removed some channels
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="422">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -1261,25 +1261,37 @@
     <t xml:space="preserve">1702587195889919_231214_155316_round4</t>
   </si>
   <si>
-    <t xml:space="preserve">1, 14, 23, 16, 8, 29, 17</t>
+    <t xml:space="preserve">1, 14, 23, 16, 8, 29</t>
   </si>
   <si>
     <t xml:space="preserve">1702932267299951_231218_154428_round1</t>
   </si>
   <si>
+    <t xml:space="preserve">30, 17, 29, 2, 13, 12, 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1702935175603837_231218_163256_round2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, 20, 3, 26, 29, 21, 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1702937566118826_231218_171246_round3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorting Log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End</t>
+  </si>
+  <si>
     <t xml:space="preserve">30, 17, 29, 2, 13, 12, 3, 31</t>
   </si>
   <si>
-    <t xml:space="preserve">1702935175603837_231218_163256_round2</t>
-  </si>
-  <si>
     <t xml:space="preserve">14, 2, 20, 3, 26, 29, 21, 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1702937566118826_231218_171246_round3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorting Log</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1302,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1344,13 +1356,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1468,7 +1473,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1717,10 +1722,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1787,7 +1788,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF444444"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1804,7 +1805,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2081,7 +2082,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2329,7 +2330,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2354,7 +2355,7 @@
       <selection pane="topRight" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -4068,11 +4069,11 @@
   </sheetPr>
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -5065,11 +5066,11 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -6505,7 +6506,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="n">
         <v>45271</v>
       </c>
@@ -6515,7 +6516,7 @@
       <c r="C83" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="D83" s="62" t="s">
+      <c r="D83" s="0" t="s">
         <v>397</v>
       </c>
       <c r="E83" s="0" t="s">
@@ -6683,17 +6684,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6701,7 +6703,15 @@
         <v>417</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="n">
         <v>45278</v>
       </c>
@@ -6711,8 +6721,14 @@
       <c r="C4" s="0" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="5" t="n">
+        <v>45383</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>45278</v>
       </c>
@@ -6720,7 +6736,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>413</v>
+        <v>420</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>45383</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45383</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6731,7 +6753,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactoring single feature lin reg stuff for diff kinds of behaviors
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -10,10 +10,10 @@
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Amygdala" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Uncertain" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Folders" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Location" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Channels" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Folders" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Location" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Channels" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="InitialRegression" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="SortingLog" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="449">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -670,7 +670,7 @@
     <t xml:space="preserve">Folder Name</t>
   </si>
   <si>
-    <t xml:space="preserve">14, 7, 11, 25, 22, 9, 20, 5, 27, 12</t>
+    <t xml:space="preserve">14, 7, 11, 25, 22, 9, 20, 5, 27, 12, 18</t>
   </si>
   <si>
     <t xml:space="preserve">1695748214323644_230926_131015_round1</t>
@@ -682,7 +682,7 @@
     <t xml:space="preserve">1695752670826611_230926_142431_round2_merged</t>
   </si>
   <si>
-    <t xml:space="preserve">5, 13, 27, 20, 24, 7, 4, 12, 6, 25</t>
+    <t xml:space="preserve">5, 13, 27, 20, 24, 7, 4, 12, 6, 25, 14</t>
   </si>
   <si>
     <t xml:space="preserve">1695755745068500_230926_151545_round3_merged</t>
@@ -1279,13 +1279,94 @@
     <t xml:space="preserve">1702937566118826_231218_171246_round3</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorting Log</t>
+    <t xml:space="preserve">Original Channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorted Channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsorted Channels</t>
   </si>
   <si>
     <t xml:space="preserve">Start</t>
   </si>
   <si>
     <t xml:space="preserve">End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14, 11, 25, 22, 20, 27, 12, 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, 7, 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11, 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 24, 4, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7, 14, 24, 27, 20, 2, 9, 17, 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4, 5, 6, 13, 12, 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28, 23, 31, 29, 7, 14, 3, 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6, 25, 12, 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13, 24, 3, 11, 26, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 10, 21, 7, 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17, 2, 13, 9, 22, 5, 26, 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13, 12, 19, 4, 27, 6, 26, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25, 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25, 10, 27, 21, 7, 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12, 6, 26, 13, 4, 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19, 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25, 10, 12, 28, 21, 24, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 13, 11, 25, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29, 22, 18, 20, 5, 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, 9, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 6, 25, 21, 27, 12, 26, 19, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27, 3, 21, 18, 25, 22, 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9, 28, 10, 4, 7, 11, 20, 6, 5, 26, 12, 19</t>
   </si>
   <si>
     <t xml:space="preserve">30, 17, 29, 2, 13, 12, 3, 31</t>
@@ -1473,7 +1554,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1722,6 +1803,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1801,11 +1894,11 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2078,11 +2171,11 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2324,38 +2417,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B55" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+      <selection pane="topRight" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H94"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C30" activeCellId="0" sqref="C30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -4062,18 +4132,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -4175,7 +4245,7 @@
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5046,6 +5116,1626 @@
       </c>
       <c r="C91" s="0" t="s">
         <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="54" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B4" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="54" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B7" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B9" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="54" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B12" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="57" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B17" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="57" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B21" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="60" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B23" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="61" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B24" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="57" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="54" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B30" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56" t="s">
+        <v>271</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="57" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B34" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="59" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="54" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B35" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="57" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B40" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59" t="s">
+        <v>297</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="54" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B41" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>299</v>
+      </c>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56" t="s">
+        <v>300</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="57" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B45" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59" t="s">
+        <v>312</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="54" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B46" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>314</v>
+      </c>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56" t="s">
+        <v>315</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="57" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B51" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="59" t="s">
+        <v>329</v>
+      </c>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59" t="s">
+        <v>330</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="54" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B52" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="57" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B55" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="59" t="s">
+        <v>337</v>
+      </c>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="54" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B56" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56" t="s">
+        <v>340</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="57" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B59" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="59" t="s">
+        <v>345</v>
+      </c>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59" t="s">
+        <v>346</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="54" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B62" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" s="56" t="s">
+        <v>351</v>
+      </c>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="57" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B66" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="59" t="s">
+        <v>360</v>
+      </c>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59" t="s">
+        <v>361</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="54" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B68" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>364</v>
+      </c>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56" t="s">
+        <v>365</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="57" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B73" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59" t="s">
+        <v>377</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="54" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B76" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C76" s="56" t="s">
+        <v>382</v>
+      </c>
+      <c r="D76" s="56"/>
+      <c r="E76" s="56" t="s">
+        <v>383</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B79" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="57" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B81" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="D81" s="59"/>
+      <c r="E81" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="5" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="57" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B85" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="D85" s="59"/>
+      <c r="E85" s="59" t="s">
+        <v>403</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="57" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B89" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" s="59" t="s">
+        <v>411</v>
+      </c>
+      <c r="D89" s="59"/>
+      <c r="E89" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="5" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="54" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B91" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="D91" s="56"/>
+      <c r="E91" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -5064,43 +6754,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.42"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>45195</v>
       </c>
@@ -5108,16 +6778,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>45195</v>
       </c>
@@ -5125,1556 +6789,555 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
         <v>45195</v>
       </c>
-      <c r="B4" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>45196</v>
-      </c>
-      <c r="B5" s="2" t="n">
+      <c r="B4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>45196</v>
+        <v>45198</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="54" t="n">
-        <v>45196</v>
-      </c>
-      <c r="B7" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>226</v>
-      </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>45197</v>
+        <v>45198</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="n">
-        <v>45198</v>
-      </c>
-      <c r="B9" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <v>45198</v>
+        <v>45202</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>45198</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>3</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>4</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="54" t="n">
-        <v>45198</v>
-      </c>
-      <c r="B12" s="55" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="56" t="s">
-        <v>236</v>
-      </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
-        <v>45202</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
-        <v>45202</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
-        <v>45202</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>3</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
-        <v>45202</v>
-      </c>
-      <c r="B16" s="2" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B20" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B21" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B23" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B24" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B25" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B27" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="57" t="n">
-        <v>45203</v>
-      </c>
-      <c r="B17" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>245</v>
-      </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59" t="s">
-        <v>246</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
-        <v>45203</v>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
-        <v>45203</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
-        <v>45203</v>
-      </c>
-      <c r="B20" s="2" t="n">
+      <c r="C27" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="23" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B30" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B33" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="57" t="n">
-        <v>45204</v>
-      </c>
-      <c r="B21" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="59" t="s">
-        <v>253</v>
-      </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59" t="s">
-        <v>254</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
-        <v>45204</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60" t="n">
-        <v>45205</v>
-      </c>
-      <c r="B23" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="59" t="s">
-        <v>257</v>
-      </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="0" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="61" t="n">
-        <v>45205</v>
-      </c>
-      <c r="B24" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
-        <v>45208</v>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
-        <v>45208</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
-        <v>45208</v>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="57" t="n">
-        <v>45209</v>
-      </c>
-      <c r="B28" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="C28" s="59" t="s">
-        <v>266</v>
-      </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59" t="s">
-        <v>267</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
-        <v>45209</v>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="54" t="n">
-        <v>45209</v>
-      </c>
-      <c r="B30" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>270</v>
-      </c>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56" t="s">
-        <v>271</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
-        <v>45210</v>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
-        <v>45210</v>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
-        <v>45210</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>3</v>
-      </c>
       <c r="C33" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="57" t="n">
-        <v>45223</v>
-      </c>
-      <c r="B34" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="59" t="s">
-        <v>278</v>
-      </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59" t="s">
-        <v>279</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="54" t="n">
-        <v>45223</v>
-      </c>
-      <c r="B35" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C35" s="56" t="s">
-        <v>281</v>
-      </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56" t="s">
-        <v>282</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
-        <v>45226</v>
+        <v>45255</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
-        <v>45226</v>
-      </c>
-      <c r="B37" s="2" t="n">
-        <v>2</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B37" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
-        <v>45226</v>
+        <v>45257</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
-        <v>45226</v>
-      </c>
-      <c r="B39" s="2" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B39" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B41" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="57" t="n">
-        <v>45229</v>
-      </c>
-      <c r="B40" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="59" t="s">
-        <v>296</v>
-      </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59" t="s">
-        <v>297</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="54" t="n">
-        <v>45229</v>
-      </c>
-      <c r="B41" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C41" s="56" t="s">
-        <v>299</v>
-      </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56" t="s">
-        <v>300</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
-        <v>45230</v>
-      </c>
-      <c r="B42" s="2" t="n">
-        <v>1</v>
+      <c r="C41" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B42" s="9" t="n">
+        <v>4</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
-        <v>45230</v>
+        <v>45267</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="n">
-        <v>45230</v>
+        <v>45267</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="57" t="n">
-        <v>45237</v>
-      </c>
-      <c r="B45" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="59" t="s">
-        <v>311</v>
-      </c>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59" t="s">
-        <v>312</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="54" t="n">
-        <v>45237</v>
-      </c>
-      <c r="B46" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C46" s="56" t="s">
-        <v>314</v>
-      </c>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56" t="s">
-        <v>315</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B46" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
-        <v>45238</v>
+        <v>45271</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
-        <v>45238</v>
+        <v>45271</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
-        <v>45238</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>3</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B49" s="9" t="n">
+        <v>4</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="n">
-        <v>45238</v>
+        <v>45274</v>
       </c>
       <c r="B50" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B52" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="57" t="n">
-        <v>45241</v>
-      </c>
-      <c r="B51" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="59" t="s">
-        <v>329</v>
-      </c>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59" t="s">
-        <v>330</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="54" t="n">
-        <v>45241</v>
-      </c>
-      <c r="B52" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C52" s="56" t="s">
-        <v>331</v>
-      </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56" t="s">
-        <v>332</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
-        <v>45242</v>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
-        <v>45242</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="57" t="n">
-        <v>45247</v>
-      </c>
-      <c r="B55" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="59" t="s">
-        <v>337</v>
-      </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59" t="s">
-        <v>338</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="54" t="n">
-        <v>45247</v>
-      </c>
-      <c r="B56" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C56" s="56" t="s">
-        <v>339</v>
-      </c>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56" t="s">
-        <v>340</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
-        <v>45250</v>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
-        <v>45250</v>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="57" t="n">
-        <v>45252</v>
-      </c>
-      <c r="B59" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C59" s="59" t="s">
-        <v>345</v>
-      </c>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59" t="s">
-        <v>346</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
-        <v>45252</v>
-      </c>
-      <c r="B60" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
-        <v>45252</v>
-      </c>
-      <c r="B61" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="54" t="n">
-        <v>45252</v>
-      </c>
-      <c r="B62" s="55" t="n">
-        <v>4</v>
-      </c>
-      <c r="C62" s="56" t="s">
-        <v>351</v>
-      </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56" t="s">
-        <v>352</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
-        <v>45255</v>
-      </c>
-      <c r="B63" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
-        <v>45255</v>
-      </c>
-      <c r="B64" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
-        <v>45255</v>
-      </c>
-      <c r="B65" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="57" t="n">
-        <v>45257</v>
-      </c>
-      <c r="B66" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" s="59" t="s">
-        <v>360</v>
-      </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59" t="s">
-        <v>361</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
-        <v>45257</v>
-      </c>
-      <c r="B67" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="54" t="n">
-        <v>45257</v>
-      </c>
-      <c r="B68" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="C68" s="56" t="s">
-        <v>364</v>
-      </c>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56" t="s">
-        <v>365</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="n">
-        <v>45258</v>
-      </c>
-      <c r="B69" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="n">
-        <v>45258</v>
-      </c>
-      <c r="B70" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
-        <v>45258</v>
-      </c>
-      <c r="B71" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
-        <v>45258</v>
-      </c>
-      <c r="B72" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="57" t="n">
-        <v>45265</v>
-      </c>
-      <c r="B73" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" s="59" t="s">
-        <v>376</v>
-      </c>
-      <c r="D73" s="59"/>
-      <c r="E73" s="59" t="s">
-        <v>377</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
-        <v>45265</v>
-      </c>
-      <c r="B74" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="n">
-        <v>45265</v>
-      </c>
-      <c r="B75" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="54" t="n">
-        <v>45265</v>
-      </c>
-      <c r="B76" s="55" t="n">
-        <v>4</v>
-      </c>
-      <c r="C76" s="56" t="s">
-        <v>382</v>
-      </c>
-      <c r="D76" s="56"/>
-      <c r="E76" s="56" t="s">
-        <v>383</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="n">
-        <v>45267</v>
-      </c>
-      <c r="B77" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="n">
-        <v>45267</v>
-      </c>
-      <c r="B78" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="n">
-        <v>45267</v>
-      </c>
-      <c r="B79" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="F79" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="n">
-        <v>45267</v>
-      </c>
-      <c r="B80" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="57" t="n">
-        <v>45271</v>
-      </c>
-      <c r="B81" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C81" s="59" t="s">
-        <v>392</v>
-      </c>
-      <c r="D81" s="59"/>
-      <c r="E81" s="59" t="s">
-        <v>393</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="n">
-        <v>45271</v>
-      </c>
-      <c r="B82" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="n">
-        <v>45271</v>
-      </c>
-      <c r="B83" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F83" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="n">
-        <v>45271</v>
-      </c>
-      <c r="B84" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="F84" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="57" t="n">
-        <v>45274</v>
-      </c>
-      <c r="B85" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C85" s="59" t="s">
-        <v>402</v>
-      </c>
-      <c r="D85" s="59"/>
-      <c r="E85" s="59" t="s">
-        <v>403</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="n">
-        <v>45274</v>
-      </c>
-      <c r="B86" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="F86" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="n">
-        <v>45274</v>
-      </c>
-      <c r="B87" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="n">
-        <v>45274</v>
-      </c>
-      <c r="B88" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="F88" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="57" t="n">
-        <v>45278</v>
-      </c>
-      <c r="B89" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C89" s="59" t="s">
-        <v>411</v>
-      </c>
-      <c r="D89" s="59"/>
-      <c r="E89" s="59" t="s">
-        <v>412</v>
-      </c>
-      <c r="F89" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="n">
-        <v>45278</v>
-      </c>
-      <c r="B90" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="F90" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="54" t="n">
-        <v>45278</v>
-      </c>
-      <c r="B91" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="C91" s="56" t="s">
-        <v>415</v>
-      </c>
-      <c r="D91" s="56"/>
-      <c r="E91" s="56" t="s">
-        <v>416</v>
-      </c>
-      <c r="F91" s="0" t="s">
-        <v>195</v>
+      <c r="C52" s="0" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6684,97 +7347,578 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>216</v>
+      </c>
       <c r="D3" s="0" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="n">
-        <v>45278</v>
-      </c>
-      <c r="B4" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>45383</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45383</v>
+      <c r="A4" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>427</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="62" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B9" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="54" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B12" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="57" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B17" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="57" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B21" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="60" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B23" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="61" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B24" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="62"/>
+      <c r="C36" s="63"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="62"/>
+      <c r="C37" s="63"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="62"/>
+      <c r="C38" s="63"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="62"/>
+      <c r="C39" s="63"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="62"/>
+      <c r="C40" s="63"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="62" t="n">
         <v>45278</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="B41" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="64"/>
+      <c r="D41" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5" t="n">
         <v>45383</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="G41" s="5" t="n">
         <v>45383</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
         <v>45278</v>
       </c>
-      <c r="B6" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="n">
+      <c r="B42" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5" t="n">
+        <v>45383</v>
+      </c>
+      <c r="G42" s="5" t="n">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="62" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B43" s="64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" s="64"/>
+      <c r="D43" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>45383</v>
+      </c>
+      <c r="G43" s="5" t="n">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="23" t="n">
         <v>45247</v>
       </c>
-      <c r="B13" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B50" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="24"/>
+      <c r="D50" s="0" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="n">
         <v>45247</v>
       </c>
-      <c r="B14" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="B51" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="0" t="s">
         <v>339</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated metadata.xlsx for sorting
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="454">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -1282,7 +1282,10 @@
     <t xml:space="preserve">Original Channels</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorted Channels</t>
+    <t xml:space="preserve">Sorted by Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorted by Julie</t>
   </si>
   <si>
     <t xml:space="preserve">Unsorted Channels</t>
@@ -1318,21 +1321,30 @@
     <t xml:space="preserve">28, 23, 31, 29, 7, 14, 3, 17</t>
   </si>
   <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29, 24, 28, 4, 11, 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19, 9, 37, 20, 5, 10, 6, 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6, 25, 12, 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13, 24, 3, 11, 26, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 10, 21, 7, 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17, 2, 13, 9, 22, 5, 25</t>
+  </si>
+  <si>
     <t xml:space="preserve">ERROR</t>
   </si>
   <si>
-    <t xml:space="preserve">6, 25, 12, 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13, 24, 3, 11, 26, 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20, 10, 21, 7, 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17, 2, 13, 9, 22, 5, 26, 25</t>
-  </si>
-  <si>
     <t xml:space="preserve">13, 12, 19, 4, 27, 6, 26, 10</t>
   </si>
   <si>
@@ -1367,6 +1379,9 @@
   </si>
   <si>
     <t xml:space="preserve">9, 28, 10, 4, 7, 11, 20, 6, 5, 26, 12, 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all sorted</t>
   </si>
   <si>
     <t xml:space="preserve">30, 17, 29, 2, 13, 12, 3, 31</t>
@@ -1554,7 +1569,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1811,6 +1826,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1898,7 +1925,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2175,7 +2202,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2425,7 +2452,7 @@
       <selection pane="topRight" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -4143,7 +4170,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -5140,7 +5167,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -6756,11 +6783,11 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -7347,21 +7374,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="32.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7386,6 +7413,9 @@
       <c r="G1" s="0" t="s">
         <v>421</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
@@ -7398,13 +7428,13 @@
         <v>214</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>422</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>424</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7418,10 +7448,10 @@
         <v>216</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>426</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7435,10 +7465,11 @@
         <v>218</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>427</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>428</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="0" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7454,8 +7485,8 @@
       <c r="D5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>429</v>
+      <c r="F5" s="0" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7471,7 +7502,7 @@
       <c r="D6" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>223</v>
       </c>
     </row>
@@ -7488,7 +7519,7 @@
       <c r="D7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="F7" s="63" t="s">
         <v>226</v>
       </c>
     </row>
@@ -7505,9 +7536,11 @@
       <c r="D8" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>64</v>
-      </c>
+      <c r="F8" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="57" t="n">
@@ -7520,11 +7553,15 @@
         <v>230</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>430</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="G9" s="65" t="n">
+        <v>45032</v>
+      </c>
+      <c r="H9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
@@ -7537,27 +7574,45 @@
         <v>232</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="G10" s="65" t="n">
+        <v>45032</v>
+      </c>
+      <c r="H10" s="65" t="n">
+        <v>45032</v>
+      </c>
+    </row>
+    <row r="11" s="64" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65" t="n">
         <v>45198</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="66" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>434</v>
+      <c r="D11" s="64" t="s">
+        <v>436</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>437</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="G11" s="65" t="n">
+        <v>45031</v>
+      </c>
+      <c r="H11" s="65" t="n">
+        <v>45032</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7573,7 +7628,7 @@
       <c r="D12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="F12" s="56" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7590,7 +7645,7 @@
       <c r="D13" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>238</v>
       </c>
     </row>
@@ -7605,10 +7660,10 @@
         <v>240</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>430</v>
+        <v>438</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7622,10 +7677,10 @@
         <v>241</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,10 +7694,10 @@
         <v>243</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7656,10 +7711,10 @@
         <v>245</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7673,10 +7728,10 @@
         <v>247</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7690,10 +7745,10 @@
         <v>249</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7707,10 +7762,10 @@
         <v>251</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7823,102 +7878,163 @@
       <c r="B35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="62"/>
-      <c r="C36" s="63"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="62"/>
-      <c r="C37" s="63"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="62"/>
-      <c r="C38" s="63"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="62"/>
-      <c r="C39" s="63"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="62"/>
-      <c r="C40" s="63"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="62" t="n">
+      <c r="A41" s="5"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5"/>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="62"/>
+      <c r="C49" s="63"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="62"/>
+      <c r="C50" s="63"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="62"/>
+      <c r="C51" s="63"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="62"/>
+      <c r="C52" s="63"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="62"/>
+      <c r="C53" s="63"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="62" t="n">
         <v>45278</v>
       </c>
-      <c r="B41" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="0" t="s">
+      <c r="B54" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="67"/>
+      <c r="D54" s="0" t="s">
         <v>411</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5" t="n">
+      <c r="F54" s="5"/>
+      <c r="G54" s="5" t="n">
         <v>45383</v>
       </c>
-      <c r="G41" s="5" t="n">
+      <c r="H54" s="5" t="n">
         <v>45383</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
+      <c r="I54" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="n">
         <v>45278</v>
       </c>
-      <c r="B42" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="0" t="s">
-        <v>447</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5" t="n">
+      <c r="B55" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5" t="n">
         <v>45383</v>
       </c>
-      <c r="G42" s="5" t="n">
+      <c r="H55" s="5" t="n">
         <v>45383</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="62" t="n">
+      <c r="I55" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="62" t="n">
         <v>45278</v>
       </c>
-      <c r="B43" s="64" t="n">
-        <v>3</v>
-      </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="0" t="s">
-        <v>448</v>
-      </c>
-      <c r="F43" s="5" t="n">
+      <c r="B56" s="67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" s="67"/>
+      <c r="D56" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="G56" s="5" t="n">
         <v>45383</v>
       </c>
-      <c r="G43" s="5" t="n">
+      <c r="H56" s="5" t="n">
         <v>45383</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="n">
+      <c r="I56" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="23" t="n">
         <v>45247</v>
       </c>
-      <c r="B50" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="0" t="s">
+      <c r="B63" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="24"/>
+      <c r="D63" s="0" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="n">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="n">
         <v>45247</v>
       </c>
-      <c r="B51" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="0" t="s">
+      <c r="B64" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="0" t="s">
         <v>339</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding simple anova results to Cortana_Recording_Metadata.xlsx
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,8 @@
     <sheet name="Channels" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="InitialRegression" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="SortingLog" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Analysis-ANOVA" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Analysis-LinReg" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="514">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -1388,6 +1390,186 @@
   </si>
   <si>
     <t xml:space="preserve">14, 2, 20, 3, 26, 29, 21, 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-09-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_027_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_002_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-09-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_024_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_011_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_010_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_020_Unit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_006_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_012_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_026_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_024_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_021_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_010_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_004_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_019_Unit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_022_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_020_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_018_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_009_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_020_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_021_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_003_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_018_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_006</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1580,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1454,6 +1636,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1493,7 +1681,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1543,6 +1731,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1569,7 +1764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1830,6 +2025,14 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1913,7 +2116,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2190,7 +2393,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2440,7 +2643,7 @@
       <selection pane="topRight" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -4158,7 +4361,7 @@
       <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -5155,7 +5358,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -6771,11 +6974,11 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -7371,7 +7574,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
@@ -8035,4 +8238,868 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.000167347651247531</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.00183374075083306</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.000272504256866232</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.0292681461802767</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.0408544513448368</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.0157046582446898</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.0370030470217893</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.00030485139103684</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.5753190717376E-006</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.00551306886663384</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.0203493517653912</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.0093569117500219</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>7.16834396218083E-012</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.00567551921407011</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.0324084567043176</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.0152606785752719</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.0108783273244698</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6.6312123780865E-012</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>7.80299610061578E-006</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.0179897142885999</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.00452884431580007</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>3.87812384813526E-006</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1.15036720241586E-005</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>5.0802631434574E-007</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>3.48005489557259E-005</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.000909303064193552</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.00137042128127269</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.0402955062172857</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.0110877305932871</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.0399456110435245</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.00862296916201926</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0.0482858559404872</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0.00239737276432677</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0.0404251274716832</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0.0213915212994397</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0.0181306288529609</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0.000371456787101544</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0.0259924251683769</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0.021951365810948</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>5.52169283538707E-007</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>4.46843053651836E-006</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>5.99143685263841E-005</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0.00818486262907165</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0.00534908622982942</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0.0183427990773176</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0.0450375913084286</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>0.0137207438451637</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>0.0308159014622524</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0.0139354605217081</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0.00408222428481898</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0.0352229638559858</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0.0113482599171506</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.0312767076889777</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0.00517590455590829</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>0.00914148375940307</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0.0368202416860903</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0.00658281460550913</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
renaming plots folder to raster_plots and creating anova_passed folder and adding plots
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,8 @@
     <sheet name="SortingLog" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Analysis-ANOVA" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Analysis-LinReg" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Analysis-PermANOVA" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Analysis-Summary" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="590">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -1570,6 +1572,234 @@
   </si>
   <si>
     <t xml:space="preserve">Channel.C_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Behavior Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-squared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coefficients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_029_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81G's attraction to Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.20625407  4.8397396 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_011_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agonism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81G's attraction to Agonism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.11196998 0.43407137]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agonism by 81G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.08138788  0.71720728]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submission by 81G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06649434 5.93678909]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06037912 1.77479039]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.04694798 2.16918303]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03029412 0.00035657]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_006_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.09869044 0.23263175]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05085822 0.18718973]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_005_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.23051073 -0.05913995]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_005_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General attraction to Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.01366736 -0.00592705]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.5339514   8.81155595]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_017_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General attraction to Affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.04928129  1.18385875]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81G's attraction to Affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.01564659 -0.07010441]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affiliation by 81G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.01766967 -0.12407418]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.12975733 3.70974324]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_027_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.45206295 25.09457591]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_019_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.08358014 2.79805871]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.04288246 -0.0209263 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.11390802 2.53350014]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.10912644 0.54626185]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05671825 0.49322349]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_022_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.0297976  0.27290256]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Agonism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2.0109226  7.70716844]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.67319624 4.81127235]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.72103399 4.37565329]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.2308383  1.38065816]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.2342799  2.71734651]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.49427986 2.67420332]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.35254217 11.78595249]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General attraction to Agonism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.55673762 4.71040136]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.08412326  8.57891216]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.04437135 15.82647129]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.16502163 3.95619344]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.97691982 -0.11304371]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinReg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PermANOVA</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1810,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1642,8 +1872,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1678,6 +1921,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FAF46"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1764,7 +2013,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2033,6 +2282,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,7 +2358,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA6A6A6"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF3FAF46"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -2116,7 +2381,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2375,6 +2640,1258 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q57"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="69" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>583</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>584</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2.2074101006976</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1.91618820713828</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2.1549031694575</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1.63436939913336</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1.50610213394371</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.14014139185557</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1.77118649519716</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2.72723767707481</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.69976597148251</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1.5901745302229</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4.02906159821023</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="66"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1.76777113757494</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1.63185608974999</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1.52138947807465</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.6793716821355</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2.54515787946982</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>4.01472539945866</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1.79469654146809</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1.44724614904559</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2.84117212159127</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2.62176931171978</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1.60624558373243</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2.50231791941221</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2.38119735532425</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1.99897224402669</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1.67433985036413</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1.94692117037371</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>1.48771520027684</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>1.70880387185988</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1.45808984198919</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>1.48586965365735</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1.87671517502119</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1.60512687967736</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>1.5812425577225</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2.08130121573154</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1.58539177480019</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>2.87319933443605</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>2.63965164315008</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1.56015382198044</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>2.34192597660081</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1.71588161330883</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>1.60345746172396</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1.77279484716295</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>1.46904572168543</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>1.44718215811966</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1.5465047856784</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>1.6694769037473</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1.80825978905348</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>1.50702991416818</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>1.64248173240046</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1.67112657224445</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>1.52503810145874</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1.83132158328407</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>1.70084982084048</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>1.7452039589713</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1.50025155234275</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>587</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>589</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2393,7 +3910,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -2643,7 +4160,7 @@
       <selection pane="topRight" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -4357,11 +5874,11 @@
   </sheetPr>
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -5354,11 +6871,11 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -6974,11 +8491,11 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -7574,7 +9091,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
@@ -8245,17 +9762,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
   </cols>
   <sheetData>
     <row r="1" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8271,6 +9789,9 @@
       <c r="D1" s="65" t="s">
         <v>455</v>
       </c>
+      <c r="E1" s="66" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -8285,6 +9806,9 @@
       <c r="D2" s="0" t="n">
         <v>0.000167347651247531</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -8299,6 +9823,9 @@
       <c r="D3" s="0" t="n">
         <v>0.00183374075083306</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -8313,6 +9840,9 @@
       <c r="D4" s="0" t="n">
         <v>0.000272504256866232</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -8327,6 +9857,9 @@
       <c r="D5" s="0" t="n">
         <v>0.0292681461802767</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -8341,6 +9874,9 @@
       <c r="D6" s="0" t="n">
         <v>0.0408544513448368</v>
       </c>
+      <c r="E6" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -8355,6 +9891,9 @@
       <c r="D7" s="0" t="n">
         <v>0.0157046582446898</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -8369,6 +9908,9 @@
       <c r="D8" s="0" t="n">
         <v>0.0370030470217893</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -8383,6 +9925,9 @@
       <c r="D9" s="0" t="n">
         <v>0.00030485139103684</v>
       </c>
+      <c r="E9" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -8397,6 +9942,9 @@
       <c r="D10" s="0" t="n">
         <v>1.5753190717376E-006</v>
       </c>
+      <c r="E10" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -8411,6 +9959,9 @@
       <c r="D11" s="0" t="n">
         <v>0.00551306886663384</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -8425,19 +9976,25 @@
       <c r="D12" s="0" t="n">
         <v>0.0203493517653912</v>
       </c>
+      <c r="E12" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="67" t="s">
         <v>465</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="67" t="s">
         <v>469</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="67" t="n">
         <v>0.0093569117500219</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8453,6 +10010,9 @@
       <c r="D14" s="0" t="n">
         <v>7.16834396218083E-012</v>
       </c>
+      <c r="E14" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -8467,6 +10027,9 @@
       <c r="D15" s="0" t="n">
         <v>0.00567551921407011</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -8481,6 +10044,9 @@
       <c r="D16" s="0" t="n">
         <v>0.0324084567043176</v>
       </c>
+      <c r="E16" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -8495,6 +10061,9 @@
       <c r="D17" s="0" t="n">
         <v>0.0152606785752719</v>
       </c>
+      <c r="E17" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -8509,19 +10078,25 @@
       <c r="D18" s="0" t="n">
         <v>0.0108783273244698</v>
       </c>
+      <c r="E18" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="67" t="s">
         <v>474</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="67" t="s">
         <v>475</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="67" t="n">
         <v>6.6312123780865E-012</v>
+      </c>
+      <c r="E19" s="67" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8537,6 +10112,9 @@
       <c r="D20" s="0" t="n">
         <v>7.80299610061578E-006</v>
       </c>
+      <c r="E20" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -8551,6 +10129,9 @@
       <c r="D21" s="0" t="n">
         <v>0.0179897142885999</v>
       </c>
+      <c r="E21" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -8565,6 +10146,9 @@
       <c r="D22" s="0" t="n">
         <v>0.00452884431580007</v>
       </c>
+      <c r="E22" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -8579,6 +10163,9 @@
       <c r="D23" s="0" t="n">
         <v>3.87812384813526E-006</v>
       </c>
+      <c r="E23" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -8593,6 +10180,9 @@
       <c r="D24" s="0" t="n">
         <v>1.15036720241586E-005</v>
       </c>
+      <c r="E24" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -8607,6 +10197,9 @@
       <c r="D25" s="0" t="n">
         <v>5.0802631434574E-007</v>
       </c>
+      <c r="E25" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -8621,6 +10214,9 @@
       <c r="D26" s="0" t="n">
         <v>3.48005489557259E-005</v>
       </c>
+      <c r="E26" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -8635,6 +10231,9 @@
       <c r="D27" s="0" t="n">
         <v>0.000909303064193552</v>
       </c>
+      <c r="E27" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -8649,6 +10248,9 @@
       <c r="D28" s="0" t="n">
         <v>0.00137042128127269</v>
       </c>
+      <c r="E28" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -8663,6 +10265,9 @@
       <c r="D29" s="0" t="n">
         <v>0.0402955062172857</v>
       </c>
+      <c r="E29" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -8677,6 +10282,9 @@
       <c r="D30" s="0" t="n">
         <v>0.0110877305932871</v>
       </c>
+      <c r="E30" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -8691,6 +10299,9 @@
       <c r="D31" s="0" t="n">
         <v>0.0399456110435245</v>
       </c>
+      <c r="E31" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -8705,33 +10316,42 @@
       <c r="D32" s="0" t="n">
         <v>0.00862296916201926</v>
       </c>
+      <c r="E32" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="67" t="s">
         <v>487</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="B33" s="67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="67" t="s">
         <v>488</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="67" t="n">
         <v>0.0482858559404872</v>
       </c>
+      <c r="E33" s="67" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="67" t="s">
         <v>489</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="B34" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="67" t="s">
         <v>466</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="67" t="n">
         <v>0.00239737276432677</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8747,6 +10367,9 @@
       <c r="D35" s="0" t="n">
         <v>0.0404251274716832</v>
       </c>
+      <c r="E35" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -8761,6 +10384,9 @@
       <c r="D36" s="0" t="n">
         <v>0.0213915212994397</v>
       </c>
+      <c r="E36" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -8775,6 +10401,9 @@
       <c r="D37" s="0" t="n">
         <v>0.0181306288529609</v>
       </c>
+      <c r="E37" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -8789,19 +10418,25 @@
       <c r="D38" s="0" t="n">
         <v>0.000371456787101544</v>
       </c>
+      <c r="E38" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="67" t="s">
         <v>495</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="67" t="n">
         <v>4</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="67" t="s">
         <v>484</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="67" t="n">
         <v>0.0259924251683769</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8817,6 +10452,9 @@
       <c r="D40" s="0" t="n">
         <v>0.021951365810948</v>
       </c>
+      <c r="E40" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -8831,6 +10469,9 @@
       <c r="D41" s="0" t="n">
         <v>5.52169283538707E-007</v>
       </c>
+      <c r="E41" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -8845,6 +10486,9 @@
       <c r="D42" s="0" t="n">
         <v>4.46843053651836E-006</v>
       </c>
+      <c r="E42" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -8859,6 +10503,9 @@
       <c r="D43" s="0" t="n">
         <v>5.99143685263841E-005</v>
       </c>
+      <c r="E43" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -8873,6 +10520,9 @@
       <c r="D44" s="0" t="n">
         <v>0.00818486262907165</v>
       </c>
+      <c r="E44" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -8887,6 +10537,9 @@
       <c r="D45" s="0" t="n">
         <v>0.00534908622982942</v>
       </c>
+      <c r="E45" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -8901,6 +10554,9 @@
       <c r="D46" s="0" t="n">
         <v>0.0183427990773176</v>
       </c>
+      <c r="E46" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -8915,6 +10571,9 @@
       <c r="D47" s="0" t="n">
         <v>0.0450375913084286</v>
       </c>
+      <c r="E47" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -8929,6 +10588,9 @@
       <c r="D48" s="0" t="n">
         <v>0.0137207438451637</v>
       </c>
+      <c r="E48" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -8943,6 +10605,9 @@
       <c r="D49" s="0" t="n">
         <v>0.0308159014622524</v>
       </c>
+      <c r="E49" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -8957,6 +10622,9 @@
       <c r="D50" s="0" t="n">
         <v>0.0139354605217081</v>
       </c>
+      <c r="E50" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -8971,6 +10639,9 @@
       <c r="D51" s="0" t="n">
         <v>0.00408222428481898</v>
       </c>
+      <c r="E51" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -8985,6 +10656,9 @@
       <c r="D52" s="0" t="n">
         <v>0.0352229638559858</v>
       </c>
+      <c r="E52" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -8999,6 +10673,9 @@
       <c r="D53" s="0" t="n">
         <v>0.0113482599171506</v>
       </c>
+      <c r="E53" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -9013,6 +10690,9 @@
       <c r="D54" s="0" t="n">
         <v>0.0312767076889777</v>
       </c>
+      <c r="E54" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
@@ -9027,6 +10707,9 @@
       <c r="D55" s="0" t="n">
         <v>0.00517590455590829</v>
       </c>
+      <c r="E55" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -9041,6 +10724,9 @@
       <c r="D56" s="0" t="n">
         <v>0.00914148375940307</v>
       </c>
+      <c r="E56" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
@@ -9055,6 +10741,9 @@
       <c r="D57" s="0" t="n">
         <v>0.0368202416860903</v>
       </c>
+      <c r="E57" s="0" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
@@ -9068,6 +10757,9 @@
       </c>
       <c r="D58" s="0" t="n">
         <v>0.00658281460550913</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -9086,14 +10778,1083 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="26.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="37.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>514</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>515</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1" s="65" t="s">
+        <v>518</v>
+      </c>
+      <c r="I1" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.787376130022259</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.00141302462633323</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.714149977396184</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.00412742172835764</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.72507271030454</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.00358126617515756</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.734398082547392</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.00315892887014564</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.737640600753071</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.00302108700727468</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.715588361621035</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.00405219461072609</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.784349723093875</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.00148681503277446</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.730766294167097</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.00331876839660095</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.846114075952503</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.000443570824989244</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.707474625239755</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.00449016011444848</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.785878208761381</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.00144920361429895</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.780344297275339</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.00158876527841905</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.707129353187573</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.00450954256313961</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.803988782853755</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.00105462762655855</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.763699249257595</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.00206810438085801</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="67" t="s">
+        <v>465</v>
+      </c>
+      <c r="B17" s="67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>469</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>520</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>542</v>
+      </c>
+      <c r="F17" s="67" t="n">
+        <v>0.881204837525589</v>
+      </c>
+      <c r="G17" s="67" t="n">
+        <v>0.000176549182897429</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>553</v>
+      </c>
+      <c r="I17" s="67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.707101280411521</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0.00451112119911595</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.751328262794826</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0.00248752021453756</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0.749550371405668</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0.00255256196778632</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="67" t="s">
+        <v>474</v>
+      </c>
+      <c r="B21" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>475</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>546</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>549</v>
+      </c>
+      <c r="F21" s="67" t="n">
+        <v>0.720424149392981</v>
+      </c>
+      <c r="G21" s="67" t="n">
+        <v>0.0038067080589425</v>
+      </c>
+      <c r="H21" s="67" t="s">
+        <v>559</v>
+      </c>
+      <c r="I21" s="67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0.707149139381861</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0.00450843015836554</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0.832865788003454</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0.000595776942024419</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0.74158029584605</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0.0028596364130994</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="67" t="s">
+        <v>487</v>
+      </c>
+      <c r="B25" s="67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>488</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="F25" s="67" t="n">
+        <v>0.735073400638693</v>
+      </c>
+      <c r="G25" s="67" t="n">
+        <v>0.00312984579624553</v>
+      </c>
+      <c r="H25" s="67" t="s">
+        <v>566</v>
+      </c>
+      <c r="I25" s="67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="67" t="s">
+        <v>489</v>
+      </c>
+      <c r="B26" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="67" t="s">
+        <v>466</v>
+      </c>
+      <c r="D26" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="F26" s="67" t="n">
+        <v>0.711185571486803</v>
+      </c>
+      <c r="G26" s="67" t="n">
+        <v>0.00428571572931137</v>
+      </c>
+      <c r="H26" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="I26" s="67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.72106861365433</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0.00377484369911458</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="67" t="s">
+        <v>495</v>
+      </c>
+      <c r="B28" s="67" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>484</v>
+      </c>
+      <c r="D28" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>525</v>
+      </c>
+      <c r="F28" s="67" t="n">
+        <v>0.737807282466348</v>
+      </c>
+      <c r="G28" s="67" t="n">
+        <v>0.0030141233437616</v>
+      </c>
+      <c r="H28" s="67" t="s">
+        <v>570</v>
+      </c>
+      <c r="I28" s="67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0.733031250915402</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0.00321840215280912</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.723125387871428</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0.00367446840750216</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>572</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0.713139104979482</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0.0041809052804653</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>575</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.807758238850952</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.000983606536464546</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>576</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.769683282494715</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.0018850560139879</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>578</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0.727748137795628</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0.00345607911942881</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.741751688201506</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0.00285276032610502</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0.807996431921935</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0.000979239335847504</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
png files and excel files
</commit_message>
<xml_diff>
--- a/resources/Cortana_Recording_Metadata.xlsx
+++ b/resources/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,8 @@
     <sheet name="Analysis-LinReg" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Analysis-PermANOVA" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Analysis-Summary" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Cells_fromEd" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="excluded" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="612">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -1800,15 +1802,82 @@
   </si>
   <si>
     <t xml:space="preserve">PermANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Window Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Window End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_014_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_009_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_004_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_013_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_025_Unit 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_019_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_004_Unit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_009_Unit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_003_Unit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel.C_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -2013,7 +2082,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2298,6 +2367,18 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2381,7 +2462,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2654,11 +2735,11 @@
   </sheetPr>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
@@ -3836,7 +3917,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -3886,6 +3967,2598 @@
       </c>
       <c r="D4" s="0" t="n">
         <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H121"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>591</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="66" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B2" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>457</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>593</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B4" s="72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>459</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B5" s="72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>480</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>594</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F6" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="71" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>554</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="F7" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>466</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>650</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>595</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>596</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>556</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F11" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="72" t="s">
+        <v>457</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F12" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>463</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>597</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="71" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="72" t="s">
+        <v>457</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F15" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>475</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>598</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="72" t="s">
+        <v>476</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F18" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>480</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="72" t="s">
+        <v>479</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F20" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>478</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F21" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>481</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>477</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F23" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>459</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F24" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>595</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F25" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="72" t="s">
+        <v>599</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="72" t="s">
+        <v>480</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F27" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="72" t="s">
+        <v>600</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F28" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>600</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>601</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F30" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>486</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F31" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="72" t="s">
+        <v>482</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F32" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="72" t="s">
+        <v>563</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F33" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="72" t="s">
+        <v>597</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F34" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="71" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>457</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F35" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="71" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="72" t="s">
+        <v>484</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F36" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="71" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F37" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="71" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="72" t="s">
+        <v>585</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F38" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="73" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" s="72" t="s">
+        <v>602</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F39" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="72" t="s">
+        <v>466</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F40" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="72" t="s">
+        <v>560</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F41" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="72" t="s">
+        <v>488</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="72" t="s">
+        <v>490</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F43" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" s="72" t="s">
+        <v>466</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F44" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="72" t="s">
+        <v>492</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F45" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="73" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="72" t="s">
+        <v>506</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F46" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="72" t="s">
+        <v>494</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F47" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="72" t="s">
+        <v>560</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F48" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F49" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F51" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F52" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="73" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F53" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="73" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="73" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="73" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="73" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" s="72" t="s">
+        <v>602</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C80" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C82" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C84" s="72" t="s">
+        <v>490</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C85" s="72" t="s">
+        <v>506</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C86" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C88" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>1750</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C93" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="73" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C95" s="72" t="s">
+        <v>610</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="73" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="73" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C97" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="73" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C98" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="73" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C99" s="72" t="s">
+        <v>491</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="73" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C100" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="73" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C101" s="72" t="s">
+        <v>573</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="73" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C102" s="72" t="s">
+        <v>573</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="73" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C103" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="73" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C104" s="72" t="s">
+        <v>602</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="73" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C105" s="72" t="s">
+        <v>505</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="73" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C106" s="72" t="s">
+        <v>602</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="72" t="s">
+        <v>606</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" s="72" t="s">
+        <v>610</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" s="72" t="s">
+        <v>510</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G110" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C111" s="72" t="s">
+        <v>484</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C112" s="72" t="s">
+        <v>513</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C113" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F113" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C114" s="72" t="s">
+        <v>560</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F114" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C115" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G115" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C116" s="72" t="s">
+        <v>490</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F116" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C117" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F117" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="73" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C118" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F118" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="73" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F119" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="73" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F120" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="73" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="73" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>498</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +6583,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -4154,13 +6827,13 @@
   </sheetPr>
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B55" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
-      <selection pane="topRight" activeCell="C91" activeCellId="0" sqref="C91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -5878,7 +8551,7 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -6875,7 +9548,7 @@
       <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -8495,7 +11168,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -9091,7 +11764,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
@@ -9768,7 +12441,7 @@
       <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.39"/>
@@ -10784,7 +13457,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>

</xml_diff>